<commit_message>
Fixed the state descriptions to be more accurate.
</commit_message>
<xml_diff>
--- a/hw/1/State_descriptions.xlsx
+++ b/hw/1/State_descriptions.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
   <si>
     <t>States</t>
   </si>
@@ -60,41 +60,51 @@
     <t>Error State</t>
   </si>
   <si>
-    <t>Start State</t>
-  </si>
-  <si>
-    <t>Man can cross with the goat</t>
-  </si>
-  <si>
     <t>Man can cross with the wolf or the cabbage</t>
   </si>
   <si>
-    <t>Man can cross with the wolf</t>
-  </si>
-  <si>
-    <t>Man can cross with the cabbage</t>
-  </si>
-  <si>
-    <t>Man can cross with the goat (follwing state q3)</t>
-  </si>
-  <si>
-    <t>Man can cross with the goat (follwing state q4)</t>
-  </si>
-  <si>
-    <t>Man can cross with either the cabbage or the wolf</t>
-  </si>
-  <si>
-    <t>Man crosses with nothing</t>
-  </si>
-  <si>
-    <t>Accepting State, man crossed with goat</t>
+    <t>Man can cross with nothing</t>
+  </si>
+  <si>
+    <t>Start State; man can cross with the goat</t>
+  </si>
+  <si>
+    <t>Accepting State; man crossed with goat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Man can cross with the goat </t>
+  </si>
+  <si>
+    <t>Man can cross with the cabbage (following state 3)</t>
+  </si>
+  <si>
+    <t>Man can cross with the wolf (following state 4)</t>
+  </si>
+  <si>
+    <t>Man can cross with goat</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Note: This is based on the DFA on page 11 of </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Formal Language A Practical Introduction</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -104,6 +114,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -435,31 +453,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -467,23 +488,23 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -491,7 +512,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -499,7 +520,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -507,31 +528,31 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -541,6 +562,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>